<commit_message>
Update NB3_ear to rev3 fab
</commit_message>
<xml_diff>
--- a/audio/NB3_ear/fab/NB3_ear.xlsx
+++ b/audio/NB3_ear/fab/NB3_ear.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="NB3_power" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="NB3_power" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t xml:space="preserve">Quantity</t>
   </si>
@@ -88,10 +88,7 @@
     <t xml:space="preserve">ICS-43434 </t>
   </si>
   <si>
-    <t xml:space="preserve">Mouser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">410-ICS-43434 </t>
+    <t xml:space="preserve">C5656610</t>
   </si>
   <si>
     <t xml:space="preserve">R1,</t>
@@ -310,30 +307,136 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.23046875" defaultRowHeight="14.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="71.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="25.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="30.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="71.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="25.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="30.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.61"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="10" style="1" width="11.23"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -359,7 +462,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="n">
         <v>1</v>
       </c>
@@ -385,7 +488,7 @@
         <v>0.0012</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
         <v>2</v>
       </c>
@@ -411,7 +514,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
         <v>1</v>
       </c>
@@ -428,79 +531,79 @@
         <v>21</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="H4" s="5" t="n">
-        <v>2.2</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" s="5" t="n">
         <v>0.0007</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H6" s="5"/>
     </row>
-    <row r="7" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H7" s="5"/>
     </row>
-    <row r="8" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H9" s="5"/>
     </row>
-    <row r="10" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H13" s="5"/>
     </row>
-    <row r="14" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H14" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Arial,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Arial,Regular"Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>